<commit_message>
panilha de avaliaçao atualizada
</commit_message>
<xml_diff>
--- a/Documentação/Planilha_de_avaliação_-_2_nivel_-_2024.xlsx
+++ b/Documentação/Planilha_de_avaliação_-_2_nivel_-_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nova\Documents\Faculdade\2 semestre\ABP\API-2\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B43E75-CBE9-4BD5-9274-EB33D4D0EAA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91082DEE-7A2D-4EE3-A5BC-AA0C0F391175}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{5A79BD2C-7FB4-4CDA-88C4-C274EF65DA92}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="109">
   <si>
     <t>Curso</t>
   </si>
@@ -328,12 +328,6 @@
     <t>https://github.com/DataSolutionsGroup2</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Todos</t>
   </si>
   <si>
@@ -358,10 +352,13 @@
     <t>Isaac</t>
   </si>
   <si>
-    <t>Felippe</t>
-  </si>
-  <si>
     <t>Renan</t>
+  </si>
+  <si>
+    <t>Fellipe</t>
+  </si>
+  <si>
+    <t>git a</t>
   </si>
 </sst>
 </file>
@@ -606,7 +603,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -678,6 +675,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -735,8 +737,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1056,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD90699-6E5A-468B-B2BB-4F443F938C44}">
   <dimension ref="A1:S80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,14 +1076,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1090,11 +1092,11 @@
       <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
       <c r="F4" s="10" t="s">
         <v>3</v>
       </c>
@@ -1106,11 +1108,11 @@
       <c r="B5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="40"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="43"/>
       <c r="F5" s="12">
         <v>45372</v>
       </c>
@@ -1127,37 +1129,37 @@
       <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="36"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="39"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="31"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="34"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
@@ -1223,7 +1225,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>16</v>
@@ -1253,7 +1255,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>18</v>
@@ -1268,7 +1270,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
@@ -1283,7 +1285,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>18</v>
@@ -1298,7 +1300,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>18</v>
@@ -1324,19 +1326,19 @@
       <c r="H21" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="I21" s="43" t="s">
+      <c r="I21" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="J21" s="43"/>
-      <c r="K21" s="43"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="43"/>
-      <c r="N21" s="43"/>
-      <c r="O21" s="43"/>
-      <c r="P21" s="43"/>
-      <c r="Q21" s="43"/>
-      <c r="R21" s="43"/>
-      <c r="S21" s="43"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="46"/>
+      <c r="Q21" s="46"/>
+      <c r="R21" s="46"/>
+      <c r="S21" s="46"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -1351,19 +1353,19 @@
       <c r="H22" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="I22" s="41" t="s">
+      <c r="I22" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="41"/>
-      <c r="Q22" s="41"/>
-      <c r="R22" s="41"/>
-      <c r="S22" s="41"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="44"/>
+      <c r="Q22" s="44"/>
+      <c r="R22" s="44"/>
+      <c r="S22" s="44"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
@@ -1378,19 +1380,19 @@
       <c r="H23" s="2">
         <v>0</v>
       </c>
-      <c r="I23" s="41" t="s">
+      <c r="I23" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="J23" s="41"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
-      <c r="P23" s="41"/>
-      <c r="Q23" s="41"/>
-      <c r="R23" s="41"/>
-      <c r="S23" s="41"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="44"/>
+      <c r="P23" s="44"/>
+      <c r="Q23" s="44"/>
+      <c r="R23" s="44"/>
+      <c r="S23" s="44"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
@@ -1404,25 +1406,25 @@
       <c r="H24" s="2">
         <v>2.5</v>
       </c>
-      <c r="I24" s="41" t="s">
+      <c r="I24" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="41"/>
-      <c r="Q24" s="41"/>
-      <c r="R24" s="41"/>
-      <c r="S24" s="41"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+      <c r="L24" s="44"/>
+      <c r="M24" s="44"/>
+      <c r="N24" s="44"/>
+      <c r="O24" s="44"/>
+      <c r="P24" s="44"/>
+      <c r="Q24" s="44"/>
+      <c r="R24" s="44"/>
+      <c r="S24" s="44"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="47"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="2" t="e">
         <f>IF(SUM(C15:C24)&gt;C26,_xlfn.CONCAT("Limite é ",C26),SUM(C15:C24))</f>
         <v>#DIV/0!</v>
@@ -1438,25 +1440,25 @@
       <c r="H25" s="2">
         <v>5</v>
       </c>
-      <c r="I25" s="41" t="s">
+      <c r="I25" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="41"/>
-      <c r="Q25" s="41"/>
-      <c r="R25" s="41"/>
-      <c r="S25" s="41"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
+      <c r="N25" s="44"/>
+      <c r="O25" s="44"/>
+      <c r="P25" s="44"/>
+      <c r="Q25" s="44"/>
+      <c r="R25" s="44"/>
+      <c r="S25" s="44"/>
     </row>
     <row r="26" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="45"/>
+      <c r="B26" s="48"/>
       <c r="C26" s="8" t="e">
         <f>ROUND(SUM(C31:C86)/COUNT(C31:C86),0)</f>
         <v>#DIV/0!</v>
@@ -1472,37 +1474,37 @@
       <c r="H26" s="2">
         <v>7.5</v>
       </c>
-      <c r="I26" s="41" t="s">
+      <c r="I26" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="41"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="41"/>
-      <c r="P26" s="41"/>
-      <c r="Q26" s="41"/>
-      <c r="R26" s="41"/>
-      <c r="S26" s="41"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
+      <c r="N26" s="44"/>
+      <c r="O26" s="44"/>
+      <c r="P26" s="44"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="44"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H27" s="2">
         <v>10</v>
       </c>
-      <c r="I27" s="41" t="s">
+      <c r="I27" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="J27" s="41"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="41"/>
-      <c r="M27" s="41"/>
-      <c r="N27" s="41"/>
-      <c r="O27" s="41"/>
-      <c r="P27" s="41"/>
-      <c r="Q27" s="41"/>
-      <c r="R27" s="41"/>
-      <c r="S27" s="41"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
+      <c r="N27" s="44"/>
+      <c r="O27" s="44"/>
+      <c r="P27" s="44"/>
+      <c r="Q27" s="44"/>
+      <c r="R27" s="44"/>
+      <c r="S27" s="44"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I28" s="20"/>
@@ -1518,16 +1520,16 @@
       <c r="S28" s="20"/>
     </row>
     <row r="29" spans="1:19" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="42"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
     </row>
     <row r="30" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
@@ -1568,9 +1570,7 @@
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="E31" s="4"/>
       <c r="F31" s="27"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -1590,9 +1590,7 @@
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="E32" s="4"/>
       <c r="F32" s="27"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -1610,18 +1608,12 @@
       <c r="B33" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F33" s="27" t="s">
+      <c r="C33" s="51" t="s">
         <v>96</v>
       </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="27"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
@@ -1633,17 +1625,11 @@
         <v>28</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F34" s="27" t="s">
-        <v>100</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="27"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
@@ -1654,18 +1640,12 @@
       <c r="B35" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F35" s="27" t="s">
+      <c r="C35" s="51" t="s">
         <v>96</v>
       </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="27"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
@@ -1709,14 +1689,12 @@
       <c r="B39" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>99</v>
+      <c r="C39" s="51" t="s">
+        <v>96</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
-      <c r="F39" s="27" t="s">
-        <v>96</v>
-      </c>
+      <c r="F39" s="27"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
@@ -1755,14 +1733,10 @@
       <c r="B42" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="C42" s="4"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
-      <c r="F42" s="27" t="s">
-        <v>105</v>
-      </c>
+      <c r="F42" s="27"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
@@ -1837,7 +1811,7 @@
         <v>31</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
@@ -1845,39 +1819,35 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
         <v>72</v>
       </c>
       <c r="B49" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="C49" s="4"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
       <c r="F49" s="27"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="23" t="s">
         <v>81</v>
       </c>
       <c r="B50" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="C50" s="4"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="27"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
         <v>68</v>
       </c>
@@ -1891,10 +1861,10 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F52" s="28"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>47</v>
       </c>
@@ -1912,205 +1882,160 @@
       </c>
       <c r="F53" s="28"/>
     </row>
-    <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
         <v>29</v>
       </c>
       <c r="B54" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="F54" s="27" t="s">
+      <c r="C54" s="51" t="s">
         <v>96</v>
       </c>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="27"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
         <v>32</v>
       </c>
       <c r="B55" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F55" s="27" t="s">
-        <v>109</v>
-      </c>
+      <c r="C55" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="27"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
         <v>33</v>
       </c>
       <c r="B56" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F56" s="27" t="s">
+      <c r="C56" s="51" t="s">
         <v>96</v>
       </c>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="27"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
-    </row>
-    <row r="57" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="J56" s="30"/>
+    </row>
+    <row r="57" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
         <v>40</v>
       </c>
       <c r="B57" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C57" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F57" s="27" t="s">
+      <c r="C57" s="51" t="s">
         <v>96</v>
       </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="27"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="24" t="s">
+    <row r="58" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="31" t="s">
         <v>30</v>
       </c>
       <c r="B58" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="F58" s="27" t="s">
+      <c r="C58" s="51" t="s">
         <v>96</v>
       </c>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="27"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="24" t="s">
         <v>41</v>
       </c>
       <c r="B59" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D59" s="4" t="s">
+      <c r="C59" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="E59" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="F59" s="27" t="s">
-        <v>100</v>
-      </c>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="27"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="24" t="s">
         <v>77</v>
       </c>
       <c r="B60" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>99</v>
+      <c r="C60" s="51" t="s">
+        <v>96</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
-      <c r="F60" s="27" t="s">
-        <v>106</v>
-      </c>
+      <c r="F60" s="27"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="24" t="s">
         <v>78</v>
       </c>
       <c r="B61" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="C61" s="51"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
-      <c r="F61" s="27" t="s">
-        <v>106</v>
-      </c>
+      <c r="F61" s="27"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="24" t="s">
         <v>79</v>
       </c>
       <c r="B62" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="C62" s="51"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
-      <c r="F62" s="27" t="s">
-        <v>109</v>
-      </c>
+      <c r="F62" s="27"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="24"/>
       <c r="B63" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C63" s="4"/>
+      <c r="C63" s="51"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
       <c r="F63" s="27"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F64" s="28"/>
     </row>
     <row r="65" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -2141,9 +2066,7 @@
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
-      <c r="F66" s="27" t="s">
-        <v>107</v>
-      </c>
+      <c r="F66" s="27"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
@@ -2171,9 +2094,7 @@
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
-      <c r="F68" s="27" t="s">
-        <v>107</v>
-      </c>
+      <c r="F68" s="27"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
@@ -2198,13 +2119,13 @@
       <c r="B70" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C70" s="48" t="s">
-        <v>99</v>
+      <c r="C70" s="29" t="s">
+        <v>105</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
       <c r="F70" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
@@ -2238,7 +2159,7 @@
         <v>49</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
@@ -2256,9 +2177,7 @@
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
-      <c r="F74" s="27" t="s">
-        <v>108</v>
-      </c>
+      <c r="F74" s="27"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
@@ -2272,9 +2191,7 @@
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
-      <c r="F75" s="27" t="s">
-        <v>108</v>
-      </c>
+      <c r="F75" s="27"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
@@ -2288,9 +2205,7 @@
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
-      <c r="F76" s="27" t="s">
-        <v>108</v>
-      </c>
+      <c r="F76" s="27"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
@@ -2322,14 +2237,12 @@
       <c r="B79" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C79" s="4" t="s">
-        <v>99</v>
+      <c r="C79" s="29" t="s">
+        <v>108</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
-      <c r="F79" s="27" t="s">
-        <v>109</v>
-      </c>
+      <c r="F79" s="27"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
@@ -2377,6 +2290,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b3f78198-29fa-40dc-a64e-451b3f068329">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="cfb6d2a8-d536-4b2e-a91d-7dbf952b7065" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006795F9309C3AB34BB3D82BE70F0FEC9D" ma:contentTypeVersion="12" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="c9a1d31a48d4168ae78733f71e7b2efa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b3f78198-29fa-40dc-a64e-451b3f068329" xmlns:ns3="cfb6d2a8-d536-4b2e-a91d-7dbf952b7065" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e56f88943290b30cde4a9180a750d4bc" ns2:_="" ns3:_="">
     <xsd:import namespace="b3f78198-29fa-40dc-a64e-451b3f068329"/>
@@ -2577,7 +2501,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2586,18 +2510,18 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b3f78198-29fa-40dc-a64e-451b3f068329">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="cfb6d2a8-d536-4b2e-a91d-7dbf952b7065" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62F3817A-E4ED-420D-9EA8-49272DEE5C63}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b3f78198-29fa-40dc-a64e-451b3f068329"/>
+    <ds:schemaRef ds:uri="cfb6d2a8-d536-4b2e-a91d-7dbf952b7065"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54428317-422F-4A9F-8CA8-7347DB55D127}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2616,21 +2540,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05E6676A-7096-42F4-A415-13FD26E6D8CE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62F3817A-E4ED-420D-9EA8-49272DEE5C63}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b3f78198-29fa-40dc-a64e-451b3f068329"/>
-    <ds:schemaRef ds:uri="cfb6d2a8-d536-4b2e-a91d-7dbf952b7065"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>